<commit_message>
adds results data used for testing
</commit_message>
<xml_diff>
--- a/data-raw/2024-use-case/2024 JPE Events 3+4 Files + Plating Scheme v5 (1)/090124_JPE24_SW_E3-4_P1_SH_rerun.xlsx
+++ b/data-raw/2024-use-case/2024 JPE Events 3+4 Files + Plating Scheme v5 (1)/090124_JPE24_SW_E3-4_P1_SH_rerun.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\canfi\OneDrive\Desktop\GVL-DWR_Stuff\JPE\2024\Results\SHERLOCK\E3+4\Ots16\GrunID Inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emanuel\projects\jpe\grunID\data-raw\2024-use-case\2024 JPE Events 3+4 Files + Plating Scheme v5 (1)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A22EAD2-0E99-4B3F-9B3B-F4CEB1A6C0EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E0AB590-8C5E-4590-BBC2-15963FEC64C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5820" yWindow="3552" windowWidth="35448" windowHeight="21768" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sherlock_output" sheetId="4" r:id="rId1"/>
@@ -409,35 +409,35 @@
     <t>NTC-3</t>
   </si>
   <si>
-    <t>DNA-POS-1</t>
-  </si>
-  <si>
-    <t>DNA-POS-3</t>
-  </si>
-  <si>
-    <t>DNA-NEG-1</t>
-  </si>
-  <si>
-    <t>DNA-NEG-2</t>
-  </si>
-  <si>
-    <t>DNA-NEG-3</t>
-  </si>
-  <si>
-    <t>DNA-POS-2</t>
-  </si>
-  <si>
     <t>F1724_3_A_1</t>
   </si>
   <si>
     <t>F6124_3_A_18</t>
+  </si>
+  <si>
+    <t>POS-DNA-1</t>
+  </si>
+  <si>
+    <t>POS-DNA-2</t>
+  </si>
+  <si>
+    <t>POS-DNA-3</t>
+  </si>
+  <si>
+    <t>NEG-DNA-1</t>
+  </si>
+  <si>
+    <t>NEG-DNA-2</t>
+  </si>
+  <si>
+    <t>NEG-DNA-3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -480,8 +480,16 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -524,8 +532,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF70AD47"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF6969"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -600,11 +620,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="19" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -675,6 +710,12 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1000,17 +1041,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97603FF2-354E-4BA1-A62B-51D5C3B34E52}">
   <dimension ref="A2:AJ204"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G87" sqref="G87"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" customWidth="1"/>
+    <col min="1" max="1" width="20.5546875" customWidth="1"/>
+    <col min="2" max="2" width="12.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1018,7 +1059,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1026,7 +1067,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1034,7 +1075,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1042,7 +1083,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -1050,7 +1091,7 @@
         <v>45300</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -1058,7 +1099,7 @@
         <v>0.37351851851851853</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -1066,7 +1107,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -1074,7 +1115,7 @@
         <v>21111913</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -1082,13 +1123,13 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B13" s="4"/>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -1096,7 +1137,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -1104,12 +1145,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -1117,7 +1158,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>23</v>
       </c>
@@ -1125,53 +1166,53 @@
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>33</v>
       </c>
       <c r="B28" s="4"/>
     </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B30" s="5"/>
       <c r="C30" s="6">
         <v>1</v>
@@ -1246,7 +1287,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B31" s="6" t="s">
         <v>34</v>
       </c>
@@ -1286,7 +1327,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B32" s="6" t="s">
         <v>39</v>
       </c>
@@ -1326,7 +1367,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="33" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B33" s="6" t="s">
         <v>42</v>
       </c>
@@ -1362,7 +1403,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="34" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B34" s="6" t="s">
         <v>43</v>
       </c>
@@ -1396,7 +1437,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="35" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B35" s="6" t="s">
         <v>45</v>
       </c>
@@ -1432,7 +1473,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="36" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B36" s="6" t="s">
         <v>48</v>
       </c>
@@ -1468,7 +1509,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="37" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B37" s="6" t="s">
         <v>51</v>
       </c>
@@ -1504,7 +1545,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="38" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B38" s="6" t="s">
         <v>54</v>
       </c>
@@ -1538,7 +1579,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="39" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B39" s="6" t="s">
         <v>55</v>
       </c>
@@ -1572,7 +1613,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B40" s="6" t="s">
         <v>57</v>
       </c>
@@ -1608,7 +1649,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B41" s="6" t="s">
         <v>60</v>
       </c>
@@ -1644,7 +1685,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="42" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B42" s="6" t="s">
         <v>63</v>
       </c>
@@ -1678,7 +1719,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="43" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B43" s="6" t="s">
         <v>64</v>
       </c>
@@ -1712,7 +1753,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="44" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B44" s="6" t="s">
         <v>66</v>
       </c>
@@ -1748,7 +1789,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="45" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B45" s="6" t="s">
         <v>69</v>
       </c>
@@ -1784,7 +1825,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="46" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B46" s="6" t="s">
         <v>72</v>
       </c>
@@ -1818,13 +1859,13 @@
         <v>38</v>
       </c>
     </row>
-    <row r="48" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A48" s="11">
         <v>484530</v>
       </c>
       <c r="B48" s="4"/>
     </row>
-    <row r="50" spans="2:33" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:33" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B50" s="6" t="s">
         <v>9</v>
       </c>
@@ -1922,7 +1963,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="51" spans="2:33" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B51" s="12">
         <v>0</v>
       </c>
@@ -2020,7 +2061,7 @@
         <v>2115</v>
       </c>
     </row>
-    <row r="52" spans="2:33" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B52" s="12">
         <v>2.0833333333333333E-3</v>
       </c>
@@ -2118,7 +2159,7 @@
         <v>2207</v>
       </c>
     </row>
-    <row r="53" spans="2:33" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B53" s="12">
         <v>4.1666666666666666E-3</v>
       </c>
@@ -2216,7 +2257,7 @@
         <v>2275</v>
       </c>
     </row>
-    <row r="54" spans="2:33" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B54" s="12">
         <v>6.2499999999999995E-3</v>
       </c>
@@ -2314,7 +2355,7 @@
         <v>2438</v>
       </c>
     </row>
-    <row r="55" spans="2:33" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B55" s="12">
         <v>8.3333333333333332E-3</v>
       </c>
@@ -2412,7 +2453,7 @@
         <v>2519</v>
       </c>
     </row>
-    <row r="56" spans="2:33" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B56" s="12">
         <v>1.0416666666666666E-2</v>
       </c>
@@ -2510,7 +2551,7 @@
         <v>2502</v>
       </c>
     </row>
-    <row r="57" spans="2:33" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B57" s="12">
         <v>1.2499999999999999E-2</v>
       </c>
@@ -2608,7 +2649,7 @@
         <v>2566</v>
       </c>
     </row>
-    <row r="58" spans="2:33" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B58" s="12">
         <v>1.4583333333333332E-2</v>
       </c>
@@ -2706,7 +2747,7 @@
         <v>2756</v>
       </c>
     </row>
-    <row r="59" spans="2:33" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B59" s="12">
         <v>1.6666666666666666E-2</v>
       </c>
@@ -2804,7 +2845,7 @@
         <v>2835</v>
       </c>
     </row>
-    <row r="60" spans="2:33" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B60" s="12">
         <v>1.8749999999999999E-2</v>
       </c>
@@ -2902,7 +2943,7 @@
         <v>2814</v>
       </c>
     </row>
-    <row r="61" spans="2:33" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B61" s="12">
         <v>2.0833333333333332E-2</v>
       </c>
@@ -3000,7 +3041,7 @@
         <v>2955</v>
       </c>
     </row>
-    <row r="62" spans="2:33" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B62" s="12">
         <v>2.2916666666666669E-2</v>
       </c>
@@ -3098,7 +3139,7 @@
         <v>2982</v>
       </c>
     </row>
-    <row r="63" spans="2:33" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B63" s="12">
         <v>2.4999999999999998E-2</v>
       </c>
@@ -3196,7 +3237,7 @@
         <v>3109</v>
       </c>
     </row>
-    <row r="64" spans="2:33" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B64" s="12">
         <v>2.7083333333333334E-2</v>
       </c>
@@ -3294,7 +3335,7 @@
         <v>3132</v>
       </c>
     </row>
-    <row r="65" spans="2:33" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B65" s="12">
         <v>2.9166666666666664E-2</v>
       </c>
@@ -3392,7 +3433,7 @@
         <v>3109</v>
       </c>
     </row>
-    <row r="66" spans="2:33" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B66" s="12">
         <v>3.125E-2</v>
       </c>
@@ -3490,7 +3531,7 @@
         <v>3301</v>
       </c>
     </row>
-    <row r="67" spans="2:33" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B67" s="12">
         <v>3.3333333333333333E-2</v>
       </c>
@@ -3588,7 +3629,7 @@
         <v>3429</v>
       </c>
     </row>
-    <row r="68" spans="2:33" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B68" s="12">
         <v>3.5416666666666666E-2</v>
       </c>
@@ -3686,7 +3727,7 @@
         <v>3443</v>
       </c>
     </row>
-    <row r="69" spans="2:33" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B69" s="12">
         <v>3.7499999999999999E-2</v>
       </c>
@@ -3784,7 +3825,7 @@
         <v>3565</v>
       </c>
     </row>
-    <row r="70" spans="2:33" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B70" s="12">
         <v>3.9583333333333331E-2</v>
       </c>
@@ -3882,7 +3923,7 @@
         <v>3750</v>
       </c>
     </row>
-    <row r="71" spans="2:33" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B71" s="12">
         <v>4.1666666666666664E-2</v>
       </c>
@@ -3980,7 +4021,7 @@
         <v>3874</v>
       </c>
     </row>
-    <row r="72" spans="2:33" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B72" s="12">
         <v>4.3750000000000004E-2</v>
       </c>
@@ -4078,7 +4119,7 @@
         <v>4099</v>
       </c>
     </row>
-    <row r="73" spans="2:33" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B73" s="12">
         <v>4.5833333333333337E-2</v>
       </c>
@@ -4176,7 +4217,7 @@
         <v>4103</v>
       </c>
     </row>
-    <row r="74" spans="2:33" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B74" s="12">
         <v>4.7916666666666663E-2</v>
       </c>
@@ -4274,7 +4315,7 @@
         <v>4353</v>
       </c>
     </row>
-    <row r="75" spans="2:33" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B75" s="12">
         <v>4.9999999999999996E-2</v>
       </c>
@@ -4372,7 +4413,7 @@
         <v>4539</v>
       </c>
     </row>
-    <row r="76" spans="2:33" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B76" s="12">
         <v>5.2083333333333336E-2</v>
       </c>
@@ -4470,7 +4511,7 @@
         <v>4694</v>
       </c>
     </row>
-    <row r="77" spans="2:33" x14ac:dyDescent="0.2">
+    <row r="77" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B77" s="12">
         <v>5.4166666666666669E-2</v>
       </c>
@@ -4568,7 +4609,7 @@
         <v>4851</v>
       </c>
     </row>
-    <row r="78" spans="2:33" x14ac:dyDescent="0.2">
+    <row r="78" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B78" s="12">
         <v>5.6250000000000001E-2</v>
       </c>
@@ -4666,7 +4707,7 @@
         <v>4960</v>
       </c>
     </row>
-    <row r="79" spans="2:33" x14ac:dyDescent="0.2">
+    <row r="79" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B79" s="12">
         <v>5.8333333333333327E-2</v>
       </c>
@@ -4764,7 +4805,7 @@
         <v>5152</v>
       </c>
     </row>
-    <row r="80" spans="2:33" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B80" s="12">
         <v>6.0416666666666667E-2</v>
       </c>
@@ -4862,7 +4903,7 @@
         <v>5311</v>
       </c>
     </row>
-    <row r="81" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B81" s="12">
         <v>6.25E-2</v>
       </c>
@@ -4960,7 +5001,7 @@
         <v>5544</v>
       </c>
     </row>
-    <row r="82" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B82" s="12">
         <v>6.458333333333334E-2</v>
       </c>
@@ -5058,7 +5099,7 @@
         <v>5748</v>
       </c>
     </row>
-    <row r="83" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B83" s="12">
         <v>6.6666666666666666E-2</v>
       </c>
@@ -5156,7 +5197,7 @@
         <v>5795</v>
       </c>
     </row>
-    <row r="84" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B84" s="12">
         <v>6.8749999999999992E-2</v>
       </c>
@@ -5254,7 +5295,7 @@
         <v>6047</v>
       </c>
     </row>
-    <row r="85" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B85" s="12">
         <v>7.0833333333333331E-2</v>
       </c>
@@ -5352,7 +5393,7 @@
         <v>6037</v>
       </c>
     </row>
-    <row r="86" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B86" s="12">
         <v>7.2916666666666671E-2</v>
       </c>
@@ -5450,7 +5491,7 @@
         <v>6256</v>
       </c>
     </row>
-    <row r="87" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B87" s="12">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -5548,7 +5589,7 @@
         <v>6377</v>
       </c>
     </row>
-    <row r="88" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B88" s="12">
         <v>7.7083333333333337E-2</v>
       </c>
@@ -5646,7 +5687,7 @@
         <v>6513</v>
       </c>
     </row>
-    <row r="89" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B89" s="12">
         <v>7.9166666666666663E-2</v>
       </c>
@@ -5744,7 +5785,7 @@
         <v>6753</v>
       </c>
     </row>
-    <row r="90" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B90" s="12">
         <v>8.1250000000000003E-2</v>
       </c>
@@ -5842,7 +5883,7 @@
         <v>6879</v>
       </c>
     </row>
-    <row r="91" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B91" s="12">
         <v>8.3333333333333329E-2</v>
       </c>
@@ -5940,13 +5981,13 @@
         <v>6965</v>
       </c>
     </row>
-    <row r="93" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
         <v>108</v>
       </c>
       <c r="B93" s="4"/>
     </row>
-    <row r="95" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B95" s="6" t="s">
         <v>9</v>
       </c>
@@ -6053,7 +6094,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="96" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B96" s="12">
         <v>0</v>
       </c>
@@ -6160,7 +6201,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="97" spans="2:36" x14ac:dyDescent="0.2">
+    <row r="97" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B97" s="12">
         <v>2.0833333333333333E-3</v>
       </c>
@@ -6267,7 +6308,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="98" spans="2:36" x14ac:dyDescent="0.2">
+    <row r="98" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B98" s="12">
         <v>4.1666666666666666E-3</v>
       </c>
@@ -6374,7 +6415,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="2:36" x14ac:dyDescent="0.2">
+    <row r="99" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B99" s="12">
         <v>6.2499999999999995E-3</v>
       </c>
@@ -6481,7 +6522,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="100" spans="2:36" x14ac:dyDescent="0.2">
+    <row r="100" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B100" s="12">
         <v>8.3333333333333332E-3</v>
       </c>
@@ -6588,7 +6629,7 @@
         <v>-122</v>
       </c>
     </row>
-    <row r="101" spans="2:36" x14ac:dyDescent="0.2">
+    <row r="101" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B101" s="12">
         <v>1.0416666666666666E-2</v>
       </c>
@@ -6695,7 +6736,7 @@
         <v>-318</v>
       </c>
     </row>
-    <row r="102" spans="2:36" x14ac:dyDescent="0.2">
+    <row r="102" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B102" s="12">
         <v>1.2499999999999999E-2</v>
       </c>
@@ -6802,7 +6843,7 @@
         <v>-428</v>
       </c>
     </row>
-    <row r="103" spans="2:36" x14ac:dyDescent="0.2">
+    <row r="103" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B103" s="12">
         <v>1.4583333333333332E-2</v>
       </c>
@@ -6909,7 +6950,7 @@
         <v>-435</v>
       </c>
     </row>
-    <row r="104" spans="2:36" x14ac:dyDescent="0.2">
+    <row r="104" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B104" s="12">
         <v>1.6666666666666666E-2</v>
       </c>
@@ -7016,7 +7057,7 @@
         <v>-533</v>
       </c>
     </row>
-    <row r="105" spans="2:36" x14ac:dyDescent="0.2">
+    <row r="105" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B105" s="12">
         <v>1.8749999999999999E-2</v>
       </c>
@@ -7123,7 +7164,7 @@
         <v>-737</v>
       </c>
     </row>
-    <row r="106" spans="2:36" x14ac:dyDescent="0.2">
+    <row r="106" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B106" s="12">
         <v>2.0833333333333332E-2</v>
       </c>
@@ -7230,7 +7271,7 @@
         <v>-765</v>
       </c>
     </row>
-    <row r="107" spans="2:36" x14ac:dyDescent="0.2">
+    <row r="107" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B107" s="12">
         <v>2.2916666666666669E-2</v>
       </c>
@@ -7337,7 +7378,7 @@
         <v>-945</v>
       </c>
     </row>
-    <row r="108" spans="2:36" x14ac:dyDescent="0.2">
+    <row r="108" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B108" s="12">
         <v>2.4999999999999998E-2</v>
       </c>
@@ -7444,7 +7485,7 @@
         <v>-1002</v>
       </c>
     </row>
-    <row r="109" spans="2:36" x14ac:dyDescent="0.2">
+    <row r="109" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B109" s="12">
         <v>2.7083333333333334E-2</v>
       </c>
@@ -7551,7 +7592,7 @@
         <v>-1121</v>
       </c>
     </row>
-    <row r="110" spans="2:36" x14ac:dyDescent="0.2">
+    <row r="110" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B110" s="12">
         <v>2.9166666666666664E-2</v>
       </c>
@@ -7658,7 +7699,7 @@
         <v>-1346</v>
       </c>
     </row>
-    <row r="111" spans="2:36" x14ac:dyDescent="0.2">
+    <row r="111" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B111" s="12">
         <v>3.125E-2</v>
       </c>
@@ -7765,7 +7806,7 @@
         <v>-1331</v>
       </c>
     </row>
-    <row r="112" spans="2:36" x14ac:dyDescent="0.2">
+    <row r="112" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B112" s="12">
         <v>3.3333333333333333E-2</v>
       </c>
@@ -7872,7 +7913,7 @@
         <v>-1361</v>
       </c>
     </row>
-    <row r="113" spans="2:36" x14ac:dyDescent="0.2">
+    <row r="113" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B113" s="12">
         <v>3.5416666666666666E-2</v>
       </c>
@@ -7979,7 +8020,7 @@
         <v>-1569</v>
       </c>
     </row>
-    <row r="114" spans="2:36" x14ac:dyDescent="0.2">
+    <row r="114" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B114" s="12">
         <v>3.7499999999999999E-2</v>
       </c>
@@ -8086,7 +8127,7 @@
         <v>-1593</v>
       </c>
     </row>
-    <row r="115" spans="2:36" x14ac:dyDescent="0.2">
+    <row r="115" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B115" s="12">
         <v>3.9583333333333331E-2</v>
       </c>
@@ -8193,7 +8234,7 @@
         <v>-1553</v>
       </c>
     </row>
-    <row r="116" spans="2:36" x14ac:dyDescent="0.2">
+    <row r="116" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B116" s="12">
         <v>4.1666666666666664E-2</v>
       </c>
@@ -8300,7 +8341,7 @@
         <v>-1588</v>
       </c>
     </row>
-    <row r="117" spans="2:36" x14ac:dyDescent="0.2">
+    <row r="117" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B117" s="12">
         <v>4.3750000000000004E-2</v>
       </c>
@@ -8407,7 +8448,7 @@
         <v>-1525</v>
       </c>
     </row>
-    <row r="118" spans="2:36" x14ac:dyDescent="0.2">
+    <row r="118" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B118" s="12">
         <v>4.5833333333333337E-2</v>
       </c>
@@ -8514,7 +8555,7 @@
         <v>-1664</v>
       </c>
     </row>
-    <row r="119" spans="2:36" x14ac:dyDescent="0.2">
+    <row r="119" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B119" s="12">
         <v>4.7916666666666663E-2</v>
       </c>
@@ -8621,7 +8662,7 @@
         <v>-1574</v>
       </c>
     </row>
-    <row r="120" spans="2:36" x14ac:dyDescent="0.2">
+    <row r="120" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B120" s="12">
         <v>4.9999999999999996E-2</v>
       </c>
@@ -8728,7 +8769,7 @@
         <v>-1505</v>
       </c>
     </row>
-    <row r="121" spans="2:36" x14ac:dyDescent="0.2">
+    <row r="121" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B121" s="12">
         <v>5.2083333333333336E-2</v>
       </c>
@@ -8835,7 +8876,7 @@
         <v>-1437</v>
       </c>
     </row>
-    <row r="122" spans="2:36" x14ac:dyDescent="0.2">
+    <row r="122" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B122" s="12">
         <v>5.4166666666666669E-2</v>
       </c>
@@ -8942,7 +8983,7 @@
         <v>-1454</v>
       </c>
     </row>
-    <row r="123" spans="2:36" x14ac:dyDescent="0.2">
+    <row r="123" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B123" s="12">
         <v>5.6250000000000001E-2</v>
       </c>
@@ -9049,7 +9090,7 @@
         <v>-1491</v>
       </c>
     </row>
-    <row r="124" spans="2:36" x14ac:dyDescent="0.2">
+    <row r="124" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B124" s="12">
         <v>5.8333333333333327E-2</v>
       </c>
@@ -9156,7 +9197,7 @@
         <v>-1409</v>
       </c>
     </row>
-    <row r="125" spans="2:36" x14ac:dyDescent="0.2">
+    <row r="125" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B125" s="12">
         <v>6.0416666666666667E-2</v>
       </c>
@@ -9263,7 +9304,7 @@
         <v>-1407</v>
       </c>
     </row>
-    <row r="126" spans="2:36" x14ac:dyDescent="0.2">
+    <row r="126" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B126" s="12">
         <v>6.25E-2</v>
       </c>
@@ -9370,7 +9411,7 @@
         <v>-1333</v>
       </c>
     </row>
-    <row r="127" spans="2:36" x14ac:dyDescent="0.2">
+    <row r="127" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B127" s="12">
         <v>6.458333333333334E-2</v>
       </c>
@@ -9477,7 +9518,7 @@
         <v>-1225</v>
       </c>
     </row>
-    <row r="128" spans="2:36" x14ac:dyDescent="0.2">
+    <row r="128" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B128" s="12">
         <v>6.6666666666666666E-2</v>
       </c>
@@ -9584,7 +9625,7 @@
         <v>-1279</v>
       </c>
     </row>
-    <row r="129" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B129" s="12">
         <v>6.8749999999999992E-2</v>
       </c>
@@ -9691,7 +9732,7 @@
         <v>-1140</v>
       </c>
     </row>
-    <row r="130" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B130" s="12">
         <v>7.0833333333333331E-2</v>
       </c>
@@ -9798,7 +9839,7 @@
         <v>-1241</v>
       </c>
     </row>
-    <row r="131" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B131" s="12">
         <v>7.2916666666666671E-2</v>
       </c>
@@ -9905,7 +9946,7 @@
         <v>-1151</v>
       </c>
     </row>
-    <row r="132" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B132" s="12">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -10012,7 +10053,7 @@
         <v>-1126</v>
       </c>
     </row>
-    <row r="133" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B133" s="12">
         <v>7.7083333333333337E-2</v>
       </c>
@@ -10119,7 +10160,7 @@
         <v>-1152</v>
       </c>
     </row>
-    <row r="134" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B134" s="12">
         <v>7.9166666666666663E-2</v>
       </c>
@@ -10226,7 +10267,7 @@
         <v>-1014</v>
       </c>
     </row>
-    <row r="135" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B135" s="12">
         <v>8.1250000000000003E-2</v>
       </c>
@@ -10333,7 +10374,7 @@
         <v>-937</v>
       </c>
     </row>
-    <row r="136" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B136" s="12">
         <v>8.3333333333333329E-2</v>
       </c>
@@ -10440,13 +10481,13 @@
         <v>-919</v>
       </c>
     </row>
-    <row r="138" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A138" s="3" t="s">
         <v>109</v>
       </c>
       <c r="B138" s="4"/>
     </row>
-    <row r="140" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B140" s="5"/>
       <c r="C140" s="6">
         <v>1</v>
@@ -10521,8 +10562,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="141" spans="1:36" ht="18" x14ac:dyDescent="0.2">
-      <c r="B141" s="26" t="s">
+    <row r="141" spans="1:36" ht="19.2" x14ac:dyDescent="0.25">
+      <c r="B141" s="28" t="s">
         <v>34</v>
       </c>
       <c r="C141" s="14">
@@ -10561,8 +10602,8 @@
         <v>110</v>
       </c>
     </row>
-    <row r="142" spans="1:36" ht="27" x14ac:dyDescent="0.2">
-      <c r="B142" s="27"/>
+    <row r="142" spans="1:36" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="B142" s="29"/>
       <c r="C142" s="15">
         <v>0.66700000000000004</v>
       </c>
@@ -10599,8 +10640,8 @@
         <v>111</v>
       </c>
     </row>
-    <row r="143" spans="1:36" ht="27" x14ac:dyDescent="0.2">
-      <c r="B143" s="27"/>
+    <row r="143" spans="1:36" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="B143" s="29"/>
       <c r="C143" s="16">
         <v>7.2916666666666671E-2</v>
       </c>
@@ -10637,8 +10678,8 @@
         <v>112</v>
       </c>
     </row>
-    <row r="144" spans="1:36" ht="27" x14ac:dyDescent="0.2">
-      <c r="B144" s="28"/>
+    <row r="144" spans="1:36" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="B144" s="30"/>
       <c r="C144" s="17">
         <v>4.3032407407407408E-2</v>
       </c>
@@ -10675,8 +10716,8 @@
         <v>113</v>
       </c>
     </row>
-    <row r="145" spans="2:27" ht="18" x14ac:dyDescent="0.2">
-      <c r="B145" s="26" t="s">
+    <row r="145" spans="2:27" ht="19.2" x14ac:dyDescent="0.25">
+      <c r="B145" s="28" t="s">
         <v>39</v>
       </c>
       <c r="C145" s="14">
@@ -10715,8 +10756,8 @@
         <v>110</v>
       </c>
     </row>
-    <row r="146" spans="2:27" ht="27" x14ac:dyDescent="0.2">
-      <c r="B146" s="27"/>
+    <row r="146" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="B146" s="29"/>
       <c r="C146" s="15">
         <v>0.999</v>
       </c>
@@ -10753,8 +10794,8 @@
         <v>111</v>
       </c>
     </row>
-    <row r="147" spans="2:27" ht="27" x14ac:dyDescent="0.2">
-      <c r="B147" s="27"/>
+    <row r="147" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="B147" s="29"/>
       <c r="C147" s="16">
         <v>5.6250000000000001E-2</v>
       </c>
@@ -10791,8 +10832,8 @@
         <v>112</v>
       </c>
     </row>
-    <row r="148" spans="2:27" ht="27" x14ac:dyDescent="0.2">
-      <c r="B148" s="28"/>
+    <row r="148" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="B148" s="30"/>
       <c r="C148" s="17">
         <v>4.5034722222222219E-2</v>
       </c>
@@ -10829,8 +10870,8 @@
         <v>113</v>
       </c>
     </row>
-    <row r="149" spans="2:27" ht="18" x14ac:dyDescent="0.2">
-      <c r="B149" s="26" t="s">
+    <row r="149" spans="2:27" ht="19.2" x14ac:dyDescent="0.25">
+      <c r="B149" s="28" t="s">
         <v>42</v>
       </c>
       <c r="C149" s="14"/>
@@ -10867,8 +10908,8 @@
         <v>110</v>
       </c>
     </row>
-    <row r="150" spans="2:27" ht="27" x14ac:dyDescent="0.2">
-      <c r="B150" s="27"/>
+    <row r="150" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="B150" s="29"/>
       <c r="C150" s="15"/>
       <c r="D150" s="15"/>
       <c r="E150" s="15">
@@ -10903,8 +10944,8 @@
         <v>111</v>
       </c>
     </row>
-    <row r="151" spans="2:27" ht="27" x14ac:dyDescent="0.2">
-      <c r="B151" s="27"/>
+    <row r="151" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="B151" s="29"/>
       <c r="C151" s="15"/>
       <c r="D151" s="15"/>
       <c r="E151" s="16">
@@ -10939,8 +10980,8 @@
         <v>112</v>
       </c>
     </row>
-    <row r="152" spans="2:27" ht="27" x14ac:dyDescent="0.2">
-      <c r="B152" s="28"/>
+    <row r="152" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="B152" s="30"/>
       <c r="C152" s="18"/>
       <c r="D152" s="18"/>
       <c r="E152" s="17">
@@ -10975,8 +11016,8 @@
         <v>113</v>
       </c>
     </row>
-    <row r="153" spans="2:27" ht="18" x14ac:dyDescent="0.2">
-      <c r="B153" s="26" t="s">
+    <row r="153" spans="2:27" ht="19.2" x14ac:dyDescent="0.25">
+      <c r="B153" s="28" t="s">
         <v>43</v>
       </c>
       <c r="C153" s="14">
@@ -11011,8 +11052,8 @@
         <v>110</v>
       </c>
     </row>
-    <row r="154" spans="2:27" ht="27" x14ac:dyDescent="0.2">
-      <c r="B154" s="27"/>
+    <row r="154" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="B154" s="29"/>
       <c r="C154" s="15">
         <v>0.98</v>
       </c>
@@ -11045,8 +11086,8 @@
         <v>111</v>
       </c>
     </row>
-    <row r="155" spans="2:27" ht="27" x14ac:dyDescent="0.2">
-      <c r="B155" s="27"/>
+    <row r="155" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="B155" s="29"/>
       <c r="C155" s="16">
         <v>3.125E-2</v>
       </c>
@@ -11079,8 +11120,8 @@
         <v>112</v>
       </c>
     </row>
-    <row r="156" spans="2:27" ht="27" x14ac:dyDescent="0.2">
-      <c r="B156" s="28"/>
+    <row r="156" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="B156" s="30"/>
       <c r="C156" s="17">
         <v>1.4953703703703705E-2</v>
       </c>
@@ -11113,8 +11154,8 @@
         <v>113</v>
       </c>
     </row>
-    <row r="157" spans="2:27" ht="18" x14ac:dyDescent="0.2">
-      <c r="B157" s="26" t="s">
+    <row r="157" spans="2:27" ht="19.2" x14ac:dyDescent="0.25">
+      <c r="B157" s="28" t="s">
         <v>45</v>
       </c>
       <c r="C157" s="14">
@@ -11149,8 +11190,8 @@
         <v>110</v>
       </c>
     </row>
-    <row r="158" spans="2:27" ht="27" x14ac:dyDescent="0.2">
-      <c r="B158" s="27"/>
+    <row r="158" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="B158" s="29"/>
       <c r="C158" s="15">
         <v>0.98699999999999999</v>
       </c>
@@ -11183,8 +11224,8 @@
         <v>111</v>
       </c>
     </row>
-    <row r="159" spans="2:27" ht="27" x14ac:dyDescent="0.2">
-      <c r="B159" s="27"/>
+    <row r="159" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="B159" s="29"/>
       <c r="C159" s="16">
         <v>2.0833333333333332E-2</v>
       </c>
@@ -11217,8 +11258,8 @@
         <v>112</v>
       </c>
     </row>
-    <row r="160" spans="2:27" ht="27" x14ac:dyDescent="0.2">
-      <c r="B160" s="28"/>
+    <row r="160" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="B160" s="30"/>
       <c r="C160" s="17">
         <v>9.3402777777777772E-3</v>
       </c>
@@ -11251,8 +11292,8 @@
         <v>113</v>
       </c>
     </row>
-    <row r="161" spans="2:27" ht="18" x14ac:dyDescent="0.2">
-      <c r="B161" s="26" t="s">
+    <row r="161" spans="2:27" ht="19.2" x14ac:dyDescent="0.25">
+      <c r="B161" s="28" t="s">
         <v>48</v>
       </c>
       <c r="C161" s="14">
@@ -11287,8 +11328,8 @@
         <v>110</v>
       </c>
     </row>
-    <row r="162" spans="2:27" ht="27" x14ac:dyDescent="0.2">
-      <c r="B162" s="27"/>
+    <row r="162" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="B162" s="29"/>
       <c r="C162" s="15">
         <v>0.98899999999999999</v>
       </c>
@@ -11321,8 +11362,8 @@
         <v>111</v>
       </c>
     </row>
-    <row r="163" spans="2:27" ht="27" x14ac:dyDescent="0.2">
-      <c r="B163" s="27"/>
+    <row r="163" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="B163" s="29"/>
       <c r="C163" s="16">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -11355,8 +11396,8 @@
         <v>112</v>
       </c>
     </row>
-    <row r="164" spans="2:27" ht="27" x14ac:dyDescent="0.2">
-      <c r="B164" s="28"/>
+    <row r="164" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="B164" s="30"/>
       <c r="C164" s="17">
         <v>2.9687500000000002E-2</v>
       </c>
@@ -11389,8 +11430,8 @@
         <v>113</v>
       </c>
     </row>
-    <row r="165" spans="2:27" ht="18" x14ac:dyDescent="0.2">
-      <c r="B165" s="26" t="s">
+    <row r="165" spans="2:27" ht="19.2" x14ac:dyDescent="0.25">
+      <c r="B165" s="28" t="s">
         <v>51</v>
       </c>
       <c r="C165" s="14">
@@ -11425,8 +11466,8 @@
         <v>110</v>
       </c>
     </row>
-    <row r="166" spans="2:27" ht="27" x14ac:dyDescent="0.2">
-      <c r="B166" s="27"/>
+    <row r="166" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="B166" s="29"/>
       <c r="C166" s="15">
         <v>0.88</v>
       </c>
@@ -11459,8 +11500,8 @@
         <v>111</v>
       </c>
     </row>
-    <row r="167" spans="2:27" ht="27" x14ac:dyDescent="0.2">
-      <c r="B167" s="27"/>
+    <row r="167" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="B167" s="29"/>
       <c r="C167" s="16">
         <v>2.9166666666666664E-2</v>
       </c>
@@ -11493,8 +11534,8 @@
         <v>112</v>
       </c>
     </row>
-    <row r="168" spans="2:27" ht="27" x14ac:dyDescent="0.2">
-      <c r="B168" s="28"/>
+    <row r="168" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="B168" s="30"/>
       <c r="C168" s="17">
         <v>9.0162037037037034E-3</v>
       </c>
@@ -11527,8 +11568,8 @@
         <v>113</v>
       </c>
     </row>
-    <row r="169" spans="2:27" ht="18" x14ac:dyDescent="0.2">
-      <c r="B169" s="26" t="s">
+    <row r="169" spans="2:27" ht="19.2" x14ac:dyDescent="0.25">
+      <c r="B169" s="28" t="s">
         <v>54</v>
       </c>
       <c r="C169" s="14"/>
@@ -11561,8 +11602,8 @@
         <v>110</v>
       </c>
     </row>
-    <row r="170" spans="2:27" ht="27" x14ac:dyDescent="0.2">
-      <c r="B170" s="27"/>
+    <row r="170" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="B170" s="29"/>
       <c r="C170" s="15"/>
       <c r="D170" s="15"/>
       <c r="E170" s="15"/>
@@ -11593,8 +11634,8 @@
         <v>111</v>
       </c>
     </row>
-    <row r="171" spans="2:27" ht="27" x14ac:dyDescent="0.2">
-      <c r="B171" s="27"/>
+    <row r="171" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="B171" s="29"/>
       <c r="C171" s="15"/>
       <c r="D171" s="15"/>
       <c r="E171" s="15"/>
@@ -11625,8 +11666,8 @@
         <v>112</v>
       </c>
     </row>
-    <row r="172" spans="2:27" ht="27" x14ac:dyDescent="0.2">
-      <c r="B172" s="28"/>
+    <row r="172" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="B172" s="30"/>
       <c r="C172" s="18"/>
       <c r="D172" s="18"/>
       <c r="E172" s="18"/>
@@ -11657,8 +11698,8 @@
         <v>113</v>
       </c>
     </row>
-    <row r="173" spans="2:27" ht="18" x14ac:dyDescent="0.2">
-      <c r="B173" s="26" t="s">
+    <row r="173" spans="2:27" ht="19.2" x14ac:dyDescent="0.25">
+      <c r="B173" s="28" t="s">
         <v>55</v>
       </c>
       <c r="C173" s="14">
@@ -11693,8 +11734,8 @@
         <v>110</v>
       </c>
     </row>
-    <row r="174" spans="2:27" ht="27" x14ac:dyDescent="0.2">
-      <c r="B174" s="27"/>
+    <row r="174" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="B174" s="29"/>
       <c r="C174" s="15">
         <v>0.999</v>
       </c>
@@ -11727,8 +11768,8 @@
         <v>111</v>
       </c>
     </row>
-    <row r="175" spans="2:27" ht="27" x14ac:dyDescent="0.2">
-      <c r="B175" s="27"/>
+    <row r="175" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="B175" s="29"/>
       <c r="C175" s="16">
         <v>7.9166666666666663E-2</v>
       </c>
@@ -11761,8 +11802,8 @@
         <v>112</v>
       </c>
     </row>
-    <row r="176" spans="2:27" ht="27" x14ac:dyDescent="0.2">
-      <c r="B176" s="28"/>
+    <row r="176" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="B176" s="30"/>
       <c r="C176" s="17">
         <v>5.8460648148148144E-2</v>
       </c>
@@ -11795,8 +11836,8 @@
         <v>113</v>
       </c>
     </row>
-    <row r="177" spans="2:27" ht="18" x14ac:dyDescent="0.2">
-      <c r="B177" s="26" t="s">
+    <row r="177" spans="2:27" ht="19.2" x14ac:dyDescent="0.25">
+      <c r="B177" s="28" t="s">
         <v>57</v>
       </c>
       <c r="C177" s="14">
@@ -11831,8 +11872,8 @@
         <v>110</v>
       </c>
     </row>
-    <row r="178" spans="2:27" ht="27" x14ac:dyDescent="0.2">
-      <c r="B178" s="27"/>
+    <row r="178" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="B178" s="29"/>
       <c r="C178" s="15">
         <v>0.98699999999999999</v>
       </c>
@@ -11865,8 +11906,8 @@
         <v>111</v>
       </c>
     </row>
-    <row r="179" spans="2:27" ht="27" x14ac:dyDescent="0.2">
-      <c r="B179" s="27"/>
+    <row r="179" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="B179" s="29"/>
       <c r="C179" s="16">
         <v>7.9166666666666663E-2</v>
       </c>
@@ -11899,8 +11940,8 @@
         <v>112</v>
       </c>
     </row>
-    <row r="180" spans="2:27" ht="27" x14ac:dyDescent="0.2">
-      <c r="B180" s="28"/>
+    <row r="180" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="B180" s="30"/>
       <c r="C180" s="17">
         <v>6.7511574074074085E-2</v>
       </c>
@@ -11933,8 +11974,8 @@
         <v>113</v>
       </c>
     </row>
-    <row r="181" spans="2:27" ht="18" x14ac:dyDescent="0.2">
-      <c r="B181" s="26" t="s">
+    <row r="181" spans="2:27" ht="19.2" x14ac:dyDescent="0.25">
+      <c r="B181" s="28" t="s">
         <v>60</v>
       </c>
       <c r="C181" s="14">
@@ -11969,8 +12010,8 @@
         <v>110</v>
       </c>
     </row>
-    <row r="182" spans="2:27" ht="27" x14ac:dyDescent="0.2">
-      <c r="B182" s="27"/>
+    <row r="182" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="B182" s="29"/>
       <c r="C182" s="15">
         <v>0.99399999999999999</v>
       </c>
@@ -12003,8 +12044,8 @@
         <v>111</v>
       </c>
     </row>
-    <row r="183" spans="2:27" ht="27" x14ac:dyDescent="0.2">
-      <c r="B183" s="27"/>
+    <row r="183" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="B183" s="29"/>
       <c r="C183" s="16">
         <v>7.0833333333333331E-2</v>
       </c>
@@ -12037,8 +12078,8 @@
         <v>112</v>
       </c>
     </row>
-    <row r="184" spans="2:27" ht="27" x14ac:dyDescent="0.2">
-      <c r="B184" s="28"/>
+    <row r="184" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="B184" s="30"/>
       <c r="C184" s="17">
         <v>4.7395833333333331E-2</v>
       </c>
@@ -12071,8 +12112,8 @@
         <v>113</v>
       </c>
     </row>
-    <row r="185" spans="2:27" ht="18" x14ac:dyDescent="0.2">
-      <c r="B185" s="26" t="s">
+    <row r="185" spans="2:27" ht="19.2" x14ac:dyDescent="0.25">
+      <c r="B185" s="28" t="s">
         <v>63</v>
       </c>
       <c r="C185" s="14"/>
@@ -12105,8 +12146,8 @@
         <v>110</v>
       </c>
     </row>
-    <row r="186" spans="2:27" ht="27" x14ac:dyDescent="0.2">
-      <c r="B186" s="27"/>
+    <row r="186" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="B186" s="29"/>
       <c r="C186" s="15"/>
       <c r="D186" s="15"/>
       <c r="E186" s="15"/>
@@ -12137,8 +12178,8 @@
         <v>111</v>
       </c>
     </row>
-    <row r="187" spans="2:27" ht="27" x14ac:dyDescent="0.2">
-      <c r="B187" s="27"/>
+    <row r="187" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="B187" s="29"/>
       <c r="C187" s="15"/>
       <c r="D187" s="15"/>
       <c r="E187" s="15"/>
@@ -12169,8 +12210,8 @@
         <v>112</v>
       </c>
     </row>
-    <row r="188" spans="2:27" ht="27" x14ac:dyDescent="0.2">
-      <c r="B188" s="28"/>
+    <row r="188" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="B188" s="30"/>
       <c r="C188" s="18"/>
       <c r="D188" s="18"/>
       <c r="E188" s="18"/>
@@ -12201,8 +12242,8 @@
         <v>113</v>
       </c>
     </row>
-    <row r="189" spans="2:27" ht="18" x14ac:dyDescent="0.2">
-      <c r="B189" s="26" t="s">
+    <row r="189" spans="2:27" ht="19.2" x14ac:dyDescent="0.25">
+      <c r="B189" s="28" t="s">
         <v>64</v>
       </c>
       <c r="C189" s="14">
@@ -12237,8 +12278,8 @@
         <v>110</v>
       </c>
     </row>
-    <row r="190" spans="2:27" ht="27" x14ac:dyDescent="0.2">
-      <c r="B190" s="27"/>
+    <row r="190" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="B190" s="29"/>
       <c r="C190" s="15">
         <v>0.88800000000000001</v>
       </c>
@@ -12271,8 +12312,8 @@
         <v>111</v>
       </c>
     </row>
-    <row r="191" spans="2:27" ht="27" x14ac:dyDescent="0.2">
-      <c r="B191" s="27"/>
+    <row r="191" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="B191" s="29"/>
       <c r="C191" s="16">
         <v>5.6250000000000001E-2</v>
       </c>
@@ -12305,8 +12346,8 @@
         <v>112</v>
       </c>
     </row>
-    <row r="192" spans="2:27" ht="27" x14ac:dyDescent="0.2">
-      <c r="B192" s="28"/>
+    <row r="192" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="B192" s="30"/>
       <c r="C192" s="17">
         <v>2.5532407407407406E-2</v>
       </c>
@@ -12339,8 +12380,8 @@
         <v>113</v>
       </c>
     </row>
-    <row r="193" spans="2:27" ht="18" x14ac:dyDescent="0.2">
-      <c r="B193" s="26" t="s">
+    <row r="193" spans="2:27" ht="19.2" x14ac:dyDescent="0.25">
+      <c r="B193" s="28" t="s">
         <v>66</v>
       </c>
       <c r="C193" s="14">
@@ -12375,8 +12416,8 @@
         <v>110</v>
       </c>
     </row>
-    <row r="194" spans="2:27" ht="27" x14ac:dyDescent="0.2">
-      <c r="B194" s="27"/>
+    <row r="194" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="B194" s="29"/>
       <c r="C194" s="15">
         <v>0.96299999999999997</v>
       </c>
@@ -12409,8 +12450,8 @@
         <v>111</v>
       </c>
     </row>
-    <row r="195" spans="2:27" ht="27" x14ac:dyDescent="0.2">
-      <c r="B195" s="27"/>
+    <row r="195" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="B195" s="29"/>
       <c r="C195" s="16">
         <v>6.0416666666666667E-2</v>
       </c>
@@ -12443,8 +12484,8 @@
         <v>112</v>
       </c>
     </row>
-    <row r="196" spans="2:27" ht="27" x14ac:dyDescent="0.2">
-      <c r="B196" s="28"/>
+    <row r="196" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="B196" s="30"/>
       <c r="C196" s="17">
         <v>3.1018518518518515E-2</v>
       </c>
@@ -12477,8 +12518,8 @@
         <v>113</v>
       </c>
     </row>
-    <row r="197" spans="2:27" ht="18" x14ac:dyDescent="0.2">
-      <c r="B197" s="26" t="s">
+    <row r="197" spans="2:27" ht="19.2" x14ac:dyDescent="0.25">
+      <c r="B197" s="28" t="s">
         <v>69</v>
       </c>
       <c r="C197" s="14">
@@ -12513,8 +12554,8 @@
         <v>110</v>
       </c>
     </row>
-    <row r="198" spans="2:27" ht="27" x14ac:dyDescent="0.2">
-      <c r="B198" s="27"/>
+    <row r="198" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="B198" s="29"/>
       <c r="C198" s="15">
         <v>0.877</v>
       </c>
@@ -12547,8 +12588,8 @@
         <v>111</v>
       </c>
     </row>
-    <row r="199" spans="2:27" ht="27" x14ac:dyDescent="0.2">
-      <c r="B199" s="27"/>
+    <row r="199" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="B199" s="29"/>
       <c r="C199" s="16">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -12581,8 +12622,8 @@
         <v>112</v>
       </c>
     </row>
-    <row r="200" spans="2:27" ht="27" x14ac:dyDescent="0.2">
-      <c r="B200" s="28"/>
+    <row r="200" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="B200" s="30"/>
       <c r="C200" s="17">
         <v>3.7534722222222219E-2</v>
       </c>
@@ -12615,8 +12656,8 @@
         <v>113</v>
       </c>
     </row>
-    <row r="201" spans="2:27" ht="18" x14ac:dyDescent="0.2">
-      <c r="B201" s="26" t="s">
+    <row r="201" spans="2:27" ht="19.2" x14ac:dyDescent="0.25">
+      <c r="B201" s="28" t="s">
         <v>72</v>
       </c>
       <c r="C201" s="14"/>
@@ -12649,8 +12690,8 @@
         <v>110</v>
       </c>
     </row>
-    <row r="202" spans="2:27" ht="27" x14ac:dyDescent="0.2">
-      <c r="B202" s="27"/>
+    <row r="202" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="B202" s="29"/>
       <c r="C202" s="15"/>
       <c r="D202" s="15"/>
       <c r="E202" s="15"/>
@@ -12681,8 +12722,8 @@
         <v>111</v>
       </c>
     </row>
-    <row r="203" spans="2:27" ht="27" x14ac:dyDescent="0.2">
-      <c r="B203" s="27"/>
+    <row r="203" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="B203" s="29"/>
       <c r="C203" s="15"/>
       <c r="D203" s="15"/>
       <c r="E203" s="15"/>
@@ -12713,8 +12754,8 @@
         <v>112</v>
       </c>
     </row>
-    <row r="204" spans="2:27" ht="27" x14ac:dyDescent="0.2">
-      <c r="B204" s="28"/>
+    <row r="204" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="B204" s="30"/>
       <c r="C204" s="18"/>
       <c r="D204" s="18"/>
       <c r="E204" s="18"/>
@@ -12747,12 +12788,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="B161:B164"/>
-    <mergeCell ref="B141:B144"/>
-    <mergeCell ref="B145:B148"/>
-    <mergeCell ref="B149:B152"/>
-    <mergeCell ref="B153:B156"/>
-    <mergeCell ref="B157:B160"/>
     <mergeCell ref="B189:B192"/>
     <mergeCell ref="B193:B196"/>
     <mergeCell ref="B197:B200"/>
@@ -12763,6 +12798,12 @@
     <mergeCell ref="B177:B180"/>
     <mergeCell ref="B181:B184"/>
     <mergeCell ref="B185:B188"/>
+    <mergeCell ref="B161:B164"/>
+    <mergeCell ref="B141:B144"/>
+    <mergeCell ref="B145:B148"/>
+    <mergeCell ref="B149:B152"/>
+    <mergeCell ref="B153:B156"/>
+    <mergeCell ref="B157:B160"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -12772,18 +12813,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BC00115-01AE-47D1-A780-FD045C07B113}">
   <dimension ref="A1:Y17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Y15" sqref="Y15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.6640625" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="15.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:25" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>115</v>
       </c>
@@ -12860,12 +12901,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:25" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>34</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="C2" s="19"/>
       <c r="D2" s="22" t="s">
@@ -12894,15 +12935,15 @@
       </c>
       <c r="X2" s="19"/>
       <c r="Y2" s="24" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25" ht="15" x14ac:dyDescent="0.2">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
         <v>39</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="C3" s="19"/>
       <c r="D3" s="22" t="s">
@@ -12931,10 +12972,10 @@
       </c>
       <c r="X3" s="19"/>
       <c r="Y3" s="24" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25" ht="15" x14ac:dyDescent="0.2">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
         <v>42</v>
       </c>
@@ -12966,7 +13007,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:25" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
         <v>43</v>
       </c>
@@ -12997,7 +13038,7 @@
       <c r="X5" s="19"/>
       <c r="Y5" s="25"/>
     </row>
-    <row r="6" spans="1:25" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:25" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
         <v>45</v>
       </c>
@@ -13030,7 +13071,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="7" spans="1:25" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:25" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
         <v>48</v>
       </c>
@@ -13063,7 +13104,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:25" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
         <v>51</v>
       </c>
@@ -13096,7 +13137,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:25" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
         <v>54</v>
       </c>
@@ -13127,12 +13168,12 @@
         <v>119</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:25" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A10" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="B10" s="22" t="s">
-        <v>123</v>
+      <c r="B10" s="26" t="s">
+        <v>125</v>
       </c>
       <c r="C10" s="19"/>
       <c r="D10" s="19"/>
@@ -13158,12 +13199,12 @@
       <c r="X10" s="19"/>
       <c r="Y10" s="19"/>
     </row>
-    <row r="11" spans="1:25" ht="15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:25" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A11" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="B11" s="22" t="s">
-        <v>128</v>
+      <c r="B11" s="26" t="s">
+        <v>126</v>
       </c>
       <c r="C11" s="19"/>
       <c r="D11" s="19"/>
@@ -13187,16 +13228,16 @@
       <c r="V11" s="19"/>
       <c r="W11" s="19"/>
       <c r="X11" s="19"/>
-      <c r="Y11" s="23" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="12" spans="1:25" ht="15" x14ac:dyDescent="0.2">
+      <c r="Y11" s="26" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A12" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="B12" s="22" t="s">
-        <v>124</v>
+      <c r="B12" s="26" t="s">
+        <v>127</v>
       </c>
       <c r="C12" s="19"/>
       <c r="D12" s="19"/>
@@ -13220,11 +13261,11 @@
       <c r="V12" s="19"/>
       <c r="W12" s="19"/>
       <c r="X12" s="19"/>
-      <c r="Y12" s="23" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="13" spans="1:25" ht="15" x14ac:dyDescent="0.2">
+      <c r="Y12" s="26" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A13" s="19" t="s">
         <v>63</v>
       </c>
@@ -13251,16 +13292,16 @@
       <c r="V13" s="19"/>
       <c r="W13" s="19"/>
       <c r="X13" s="19"/>
-      <c r="Y13" s="23" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="14" spans="1:25" ht="15" x14ac:dyDescent="0.2">
+      <c r="Y13" s="26" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A14" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="B14" s="22" t="s">
-        <v>125</v>
+      <c r="B14" s="27" t="s">
+        <v>128</v>
       </c>
       <c r="C14" s="19"/>
       <c r="D14" s="19"/>
@@ -13286,12 +13327,12 @@
       <c r="X14" s="19"/>
       <c r="Y14" s="19"/>
     </row>
-    <row r="15" spans="1:25" ht="15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:25" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A15" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="B15" s="22" t="s">
-        <v>126</v>
+      <c r="B15" s="27" t="s">
+        <v>129</v>
       </c>
       <c r="C15" s="19"/>
       <c r="D15" s="19"/>
@@ -13315,16 +13356,16 @@
       <c r="V15" s="19"/>
       <c r="W15" s="19"/>
       <c r="X15" s="19"/>
-      <c r="Y15" s="23" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="16" spans="1:25" ht="15" x14ac:dyDescent="0.2">
+      <c r="Y15" s="27" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A16" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="B16" s="22" t="s">
-        <v>127</v>
+      <c r="B16" s="27" t="s">
+        <v>130</v>
       </c>
       <c r="C16" s="19"/>
       <c r="D16" s="19"/>
@@ -13348,11 +13389,11 @@
       <c r="V16" s="19"/>
       <c r="W16" s="19"/>
       <c r="X16" s="19"/>
-      <c r="Y16" s="23" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="17" spans="1:25" ht="15" x14ac:dyDescent="0.2">
+      <c r="Y16" s="27" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A17" s="19" t="s">
         <v>72</v>
       </c>
@@ -13379,8 +13420,8 @@
       <c r="V17" s="19"/>
       <c r="W17" s="19"/>
       <c r="X17" s="19"/>
-      <c r="Y17" s="23" t="s">
-        <v>127</v>
+      <c r="Y17" s="27" t="s">
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -13389,14 +13430,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a707c639-4ab7-466f-ab80-9083af4ef22b">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="02ee1384-56f9-49a7-aa58-df62156adfc7" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -13629,21 +13668,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a707c639-4ab7-466f-ab80-9083af4ef22b">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="02ee1384-56f9-49a7-aa58-df62156adfc7" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7A3C004D-50D8-40C8-AED7-5F96A76F09D6}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD573520-E05F-4496-B3C8-A0C45D49614B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="a707c639-4ab7-466f-ab80-9083af4ef22b"/>
-    <ds:schemaRef ds:uri="02ee1384-56f9-49a7-aa58-df62156adfc7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -13668,9 +13706,12 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD573520-E05F-4496-B3C8-A0C45D49614B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7A3C004D-50D8-40C8-AED7-5F96A76F09D6}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a707c639-4ab7-466f-ab80-9083af4ef22b"/>
+    <ds:schemaRef ds:uri="02ee1384-56f9-49a7-aa58-df62156adfc7"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>